<commit_message>
Feature/GDE-8193 updates for RPA S3 Close Deal
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S3_EU_NonRPA_Branch_Proc.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S3_EU_NonRPA_Branch_Proc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="7455" windowWidth="28800" windowHeight="7830" tabRatio="877" firstSheet="6" activeTab="11" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="6" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="F2" s="115" t="n"/>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D2" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="E2" s="15" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="G2" s="15" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L2" s="91" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="M2" s="91" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="D3" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="E3" s="15" t="inlineStr">
@@ -2685,8 +2685,8 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -2707,8 +2707,8 @@
     <col width="32.7109375" bestFit="1" customWidth="1" style="90" min="15" max="15"/>
     <col width="12.28515625" bestFit="1" customWidth="1" style="90" min="16" max="16"/>
     <col width="15.140625" bestFit="1" customWidth="1" style="90" min="17" max="17"/>
-    <col width="8.7109375" customWidth="1" style="90" min="18" max="48"/>
-    <col width="8.7109375" customWidth="1" style="90" min="49" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="90" min="18" max="49"/>
+    <col width="8.7109375" customWidth="1" style="90" min="50" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="85">
@@ -2811,12 +2811,12 @@
       </c>
       <c r="C2" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="E2" s="91" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="K2" s="89" t="n">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="M2" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="N2" s="90" t="inlineStr">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="G2" s="91" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="I2" s="91" t="inlineStr">
@@ -4803,7 +4803,7 @@
       </c>
       <c r="S2" s="91" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="T2" s="91" t="inlineStr">
@@ -5331,8 +5331,8 @@
     <col width="8.7109375" customWidth="1" style="63" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="63" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="63" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="67" min="46" max="97"/>
-    <col width="9.140625" customWidth="1" style="67" min="98" max="16384"/>
+    <col width="9.140625" customWidth="1" style="67" min="46" max="98"/>
+    <col width="9.140625" customWidth="1" style="67" min="99" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="60">
@@ -8678,17 +8678,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>S3_11112020115021FYP</t>
+          <t>S3_11112020195757MFL</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="H2" s="51" t="inlineStr">
@@ -9043,12 +9043,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>S3_11112020115021FYP</t>
+          <t>S3_11112020195757MFL</t>
         </is>
       </c>
       <c r="H3" s="51" t="inlineStr">
@@ -9403,12 +9403,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>S3_11112020115021FYP</t>
+          <t>S3_11112020195757MFL</t>
         </is>
       </c>
       <c r="H4" s="51" t="inlineStr">
@@ -9839,7 +9839,7 @@
       </c>
       <c r="C2" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="D2" s="123" t="inlineStr">
@@ -10099,12 +10099,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="G2" s="91" t="inlineStr">
@@ -10241,7 +10241,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="I3" s="122" t="n"/>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="I4" s="122" t="n"/>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="D2" s="123" t="inlineStr">
@@ -11141,12 +11141,12 @@
       </c>
       <c r="C2" s="90" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="E2" s="91" t="inlineStr">
@@ -11380,9 +11380,9 @@
   </sheetPr>
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF36" sqref="AF36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF21" sqref="AF21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -11662,12 +11662,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="D2" s="91" t="inlineStr">
         <is>
-          <t>OBUBRANCHPROC11112020152050CAI</t>
+          <t>OBUBRANCHPROC11112020200854YLL</t>
         </is>
       </c>
       <c r="E2" s="91" t="inlineStr">
@@ -11696,14 +11696,14 @@
         </is>
       </c>
       <c r="J2" s="91" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K2" s="91" t="n">
         <v>100</v>
       </c>
       <c r="L2" s="121" t="inlineStr">
         <is>
-          <t>12,500,000.00</t>
+          <t>15,000,000.00</t>
         </is>
       </c>
       <c r="M2" s="91" t="inlineStr">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="L3" s="45" t="n"/>
@@ -11890,7 +11890,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NONRPA BRANCH_PROC 50M11112020115018UAW</t>
+          <t>NONRPA BRANCH_PROC 50M11112020195754CRW</t>
         </is>
       </c>
       <c r="L4" s="45" t="n"/>

</xml_diff>